<commit_message>
feat: adição do prototipo
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BBBA2A-4720-438A-94DD-2AF1D8BFCBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="666" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -14,7 +15,7 @@
     <sheet name="Ver-Construção1" sheetId="3" r:id="rId5"/>
     <sheet name="Ver-Transição1" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -142,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -194,12 +195,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -311,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -344,7 +345,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -363,12 +364,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -397,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -480,7 +481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -513,7 +514,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000004000000}">
       <text>
         <r>
           <rPr>
@@ -532,12 +533,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Autor</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0" shapeId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -566,7 +567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -649,7 +650,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0" shapeId="0">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -682,7 +683,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0" shapeId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1057,7 +1058,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="17">
     <font>
       <sz val="11"/>
@@ -1384,7 +1385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1504,10 +1505,13 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1534,7 +1538,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1553,7 +1557,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1607,7 +1611,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.95833333333333337</c:v>
+                  <c:v>0.95652173913043481</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1689,7 +1693,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1863,7 +1867,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.875</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.75</c:v>
@@ -2202,7 +2206,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.125</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -2425,7 +2429,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3149,7 +3153,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3897,7 +3901,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -7290,7 +7294,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7323,7 +7327,7 @@
       </c>
       <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.95833333333333337</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7366,7 +7370,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
@@ -7743,7 +7747,7 @@
       </c>
       <c r="B10" s="25">
         <f>('Ver-Iniciação1'!$G$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="C10" s="25">
         <f>('Ver-Iniciação1'!$H$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
@@ -7755,7 +7759,7 @@
       </c>
       <c r="E10" s="25">
         <f>('Ver-Iniciação1'!$J$28/SUM('Ver-Iniciação1'!$G$28:'Ver-Iniciação1'!$J$28))</f>
-        <v>0.125</v>
+        <v>0.25</v>
       </c>
       <c r="N10" t="s">
         <v>13</v>
@@ -8404,11 +8408,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8447,7 +8451,7 @@
       <c r="E2" s="40"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.95833333333333337</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -8891,7 +8895,7 @@
       <c r="F28" s="12"/>
       <c r="G28">
         <f>COUNTIF(D29:D36,"Sim")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H28">
         <f>COUNTIF(D29:D36,"Parcialmente")</f>
@@ -8903,7 +8907,7 @@
       </c>
       <c r="J28">
         <f>COUNTIF(D29:D36,"NA")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15">
@@ -8998,7 +9002,7 @@
         <v>83</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
@@ -9011,7 +9015,7 @@
       <c r="C36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="45" t="s">
         <v>116</v>
       </c>
       <c r="E36" s="8"/>
@@ -9114,7 +9118,7 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9125,7 +9129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9798,10 +9802,10 @@
     <mergeCell ref="A5:A16"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 D22 D28 D35 D39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17 D22 D28 D35 D39" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40:D41 D36:D38 D29:D34 D18:D21 D16 D11:D14 D8:D9 D6 D23:D27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D40:D41 D36:D38 D29:D34 D18:D21 D16 D11:D14 D8:D9 D6 D23:D27" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9811,7 +9815,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10522,23 +10526,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D36:D39 D41:D42 D18:D22 D24:D28 D30:D34">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D36:D39 D41:D42 D18:D22 D24:D28 D30:D34" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10548,7 +10552,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
@@ -11301,11 +11305,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11313,12 +11312,17 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D23:D24 D26:D27 D29 D31:D35 D42:D43 D18:D21 D37:D40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D23:D24 D26:D27 D29 D31:D35 D42:D43 D18:D21 D37:D40" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Ajustes no visão, checklist e planejamento
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BBBA2A-4720-438A-94DD-2AF1D8BFCBCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FF876-0099-4A5A-B689-FCE93039BA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="118">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1053,6 +1053,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Todas as tarefas devem ser lançadas no backlog do produto no github. No sprint ficam apenas as tarefas do sprint puxadas do backlog.</t>
   </si>
 </sst>
 </file>
@@ -1454,6 +1457,9 @@
     <xf numFmtId="9" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1504,9 +1510,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1611,7 +1614,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.95652173913043481</c:v>
+                  <c:v>0.91304347826086951</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1855,7 +1858,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1968,7 +1971,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -7308,10 +7311,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="18" t="s">
@@ -7327,7 +7330,7 @@
       </c>
       <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.95652173913043481</v>
+        <v>0.91304347826086951</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7587,11 +7590,11 @@
       </c>
       <c r="B6" s="25">
         <f>('Ver-Iniciação1'!$G$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="25">
         <f>('Ver-Iniciação1'!$H$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="25">
         <f>('Ver-Iniciação1'!$I$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
@@ -8411,8 +8414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8430,41 +8433,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.95652173913043481</v>
+        <v>0.91304347826086951</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -8487,7 +8490,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
@@ -8515,7 +8518,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -8529,7 +8532,7 @@
       <c r="F6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="9"/>
@@ -8557,7 +8560,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="22">
         <v>2</v>
       </c>
@@ -8571,7 +8574,7 @@
       <c r="F8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -8585,7 +8588,7 @@
       <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>4</v>
       </c>
@@ -8599,7 +8602,7 @@
       <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="15">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>5</v>
       </c>
@@ -8613,7 +8616,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="16.5" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>6</v>
       </c>
@@ -8627,7 +8630,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>3</v>
@@ -8653,7 +8656,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="23">
         <v>7</v>
       </c>
@@ -8667,7 +8670,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="5">
         <v>8</v>
       </c>
@@ -8681,7 +8684,7 @@
       <c r="F15" s="8"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>9</v>
       </c>
@@ -8695,7 +8698,7 @@
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="15">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="23">
         <v>10</v>
       </c>
@@ -8709,7 +8712,7 @@
       <c r="F17" s="8"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="15">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -8723,7 +8726,7 @@
       <c r="F18" s="8"/>
     </row>
     <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
         <v>96</v>
@@ -8749,7 +8752,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="23">
         <v>12</v>
       </c>
@@ -8763,7 +8766,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="30">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>13</v>
       </c>
@@ -8777,7 +8780,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="9"/>
       <c r="C22" s="10" t="s">
         <v>4</v>
@@ -8787,11 +8790,11 @@
       <c r="F22" s="12"/>
       <c r="G22">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <f>COUNTIF(D23:D24,"Não")</f>
@@ -8802,8 +8805,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="31"/>
+    <row r="23" spans="1:10" ht="75">
+      <c r="A23" s="32"/>
       <c r="B23" s="23">
         <v>14</v>
       </c>
@@ -8811,13 +8814,15 @@
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -8831,7 +8836,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="15">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="9"/>
       <c r="C25" s="10" t="s">
         <v>36</v>
@@ -8857,7 +8862,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="23">
         <v>16</v>
       </c>
@@ -8871,7 +8876,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>17</v>
       </c>
@@ -8885,7 +8890,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>13</v>
@@ -8911,7 +8916,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="31"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="23">
         <v>21</v>
       </c>
@@ -8925,7 +8930,7 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="31"/>
+      <c r="A30" s="32"/>
       <c r="B30" s="5">
         <v>22</v>
       </c>
@@ -8939,7 +8944,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="31"/>
+      <c r="A31" s="32"/>
       <c r="B31" s="5">
         <v>23</v>
       </c>
@@ -8953,7 +8958,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="31"/>
+      <c r="A32" s="32"/>
       <c r="B32" s="5">
         <v>24</v>
       </c>
@@ -8967,7 +8972,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="31"/>
+      <c r="A33" s="32"/>
       <c r="B33" s="5">
         <v>25</v>
       </c>
@@ -8981,7 +8986,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="31"/>
+      <c r="A34" s="32"/>
       <c r="B34" s="5">
         <v>26</v>
       </c>
@@ -8994,7 +8999,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A35" s="31"/>
+      <c r="A35" s="32"/>
       <c r="B35" s="5">
         <v>27</v>
       </c>
@@ -9008,21 +9013,21 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="15">
-      <c r="A36" s="31"/>
+      <c r="A36" s="32"/>
       <c r="B36" s="5">
         <v>28</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="28" t="s">
         <v>116</v>
       </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:10" ht="15" customHeight="1">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B37" s="9"/>
@@ -9050,7 +9055,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="23">
         <v>30</v>
       </c>
@@ -9064,7 +9069,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5">
         <v>31</v>
       </c>
@@ -9078,7 +9083,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5">
         <v>32</v>
       </c>
@@ -9092,7 +9097,7 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="20.25" customHeight="1">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -9118,7 +9123,7 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{D862B195-455A-4EFD-824E-16CDF79502AC}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9148,41 +9153,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -9205,7 +9210,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9217,7 +9222,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -9245,7 +9250,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -9255,7 +9260,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -9283,7 +9288,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -9299,7 +9304,7 @@
       <c r="J9"/>
     </row>
     <row r="10" spans="1:10" ht="15">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10" t="s">
         <v>96</v>
@@ -9309,7 +9314,7 @@
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="23">
         <v>4</v>
       </c>
@@ -9337,7 +9342,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="23">
         <v>5</v>
       </c>
@@ -9349,7 +9354,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="30">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="5">
         <v>6</v>
       </c>
@@ -9361,7 +9366,7 @@
       <c r="F13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="30">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>7</v>
       </c>
@@ -9373,7 +9378,7 @@
       <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="15">
-      <c r="A15" s="31"/>
+      <c r="A15" s="32"/>
       <c r="B15" s="9"/>
       <c r="C15" s="10" t="s">
         <v>4</v>
@@ -9383,7 +9388,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>7</v>
       </c>
@@ -9411,7 +9416,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="9"/>
@@ -9423,7 +9428,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -9451,7 +9456,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="23">
         <v>10</v>
       </c>
@@ -9463,7 +9468,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -9475,7 +9480,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="45">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>12</v>
       </c>
@@ -9487,7 +9492,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="9"/>
@@ -9499,7 +9504,7 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="30">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="5">
         <v>17</v>
       </c>
@@ -9527,7 +9532,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>18</v>
       </c>
@@ -9539,7 +9544,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5">
         <v>19</v>
       </c>
@@ -9551,7 +9556,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5">
         <v>21</v>
       </c>
@@ -9563,7 +9568,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>22</v>
       </c>
@@ -9575,7 +9580,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="41" t="s">
+      <c r="A28" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="9"/>
@@ -9587,7 +9592,7 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="41"/>
+      <c r="A29" s="42"/>
       <c r="B29" s="5">
         <v>23</v>
       </c>
@@ -9615,7 +9620,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -9627,7 +9632,7 @@
       <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>25</v>
       </c>
@@ -9639,7 +9644,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>26</v>
       </c>
@@ -9651,7 +9656,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>27</v>
       </c>
@@ -9663,7 +9668,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>28</v>
       </c>
@@ -9675,7 +9680,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -9687,7 +9692,7 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5">
         <v>29</v>
       </c>
@@ -9715,7 +9720,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>30</v>
       </c>
@@ -9727,7 +9732,7 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>31</v>
       </c>
@@ -9739,7 +9744,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10" t="s">
         <v>15</v>
@@ -9749,7 +9754,7 @@
       <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5">
         <v>32</v>
       </c>
@@ -9777,7 +9782,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -9834,41 +9839,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -9891,7 +9896,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -9903,7 +9908,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -9931,7 +9936,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -9941,7 +9946,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -9969,7 +9974,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>96</v>
@@ -9979,7 +9984,7 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10007,7 +10012,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10019,7 +10024,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10031,7 +10036,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10041,7 +10046,7 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10069,7 +10074,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10081,7 +10086,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10109,7 +10114,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10121,7 +10126,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="15">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>11</v>
       </c>
@@ -10149,7 +10154,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="30">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5">
         <v>13</v>
       </c>
@@ -10161,7 +10166,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>14</v>
       </c>
@@ -10173,7 +10178,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="31"/>
+      <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>15</v>
       </c>
@@ -10185,7 +10190,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="32"/>
       <c r="B22" s="5">
         <v>16</v>
       </c>
@@ -10197,7 +10202,7 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="9"/>
@@ -10209,7 +10214,7 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:10" ht="30">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="23">
         <v>17</v>
       </c>
@@ -10237,7 +10242,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" ht="30">
-      <c r="A25" s="31"/>
+      <c r="A25" s="32"/>
       <c r="B25" s="5">
         <v>18</v>
       </c>
@@ -10249,7 +10254,7 @@
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="5">
         <v>19</v>
       </c>
@@ -10261,7 +10266,7 @@
       <c r="F26" s="8"/>
     </row>
     <row r="27" spans="1:10" ht="15">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>21</v>
       </c>
@@ -10273,7 +10278,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="5">
         <v>22</v>
       </c>
@@ -10285,7 +10290,7 @@
       <c r="F28" s="8"/>
     </row>
     <row r="29" spans="1:10" ht="15">
-      <c r="A29" s="41" t="s">
+      <c r="A29" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="9"/>
@@ -10297,7 +10302,7 @@
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41"/>
+      <c r="A30" s="42"/>
       <c r="B30" s="5">
         <v>24</v>
       </c>
@@ -10325,7 +10330,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="30">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>26</v>
       </c>
@@ -10337,7 +10342,7 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" spans="1:10" ht="15">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>27</v>
       </c>
@@ -10349,7 +10354,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>28</v>
       </c>
@@ -10361,7 +10366,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>29</v>
       </c>
@@ -10373,7 +10378,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15" customHeight="1">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
@@ -10385,7 +10390,7 @@
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:10" ht="30">
-      <c r="A36" s="30"/>
+      <c r="A36" s="31"/>
       <c r="B36" s="5">
         <v>30</v>
       </c>
@@ -10413,7 +10418,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>31</v>
       </c>
@@ -10425,7 +10430,7 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:10" ht="30">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>32</v>
       </c>
@@ -10437,7 +10442,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="15">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5"/>
       <c r="C39" s="8" t="s">
         <v>104</v>
@@ -10447,7 +10452,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10" t="s">
         <v>15</v>
@@ -10457,7 +10462,7 @@
       <c r="F40" s="12"/>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="5">
         <v>33</v>
       </c>
@@ -10485,7 +10490,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="30"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="5">
         <v>34</v>
       </c>
@@ -10526,17 +10531,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -10571,41 +10576,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19.5" customHeight="1">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="16"/>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="21" t="e">
         <f>COUNTIF(D5:D43,"Sim")/(COUNTA(D5:D43)-COUNTIF(D5:D43,"NA"))</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="33"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="45"/>
     </row>
     <row r="4" spans="1:10" ht="15">
       <c r="A4" s="6" t="s">
@@ -10628,7 +10633,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="35" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="9"/>
@@ -10640,7 +10645,7 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:10" ht="15">
-      <c r="A6" s="31"/>
+      <c r="A6" s="32"/>
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -10668,7 +10673,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
-      <c r="A7" s="31"/>
+      <c r="A7" s="32"/>
       <c r="B7" s="9"/>
       <c r="C7" s="10" t="s">
         <v>3</v>
@@ -10678,7 +10683,7 @@
       <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A8" s="31"/>
+      <c r="A8" s="32"/>
       <c r="B8" s="5">
         <v>2</v>
       </c>
@@ -10706,7 +10711,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
         <v>14</v>
@@ -10716,7 +10721,7 @@
       <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:10" ht="30">
-      <c r="A10" s="31"/>
+      <c r="A10" s="32"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10744,7 +10749,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
-      <c r="A11" s="31"/>
+      <c r="A11" s="32"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10756,7 +10761,7 @@
       <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="29.25" customHeight="1">
-      <c r="A12" s="31"/>
+      <c r="A12" s="32"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10768,7 +10773,7 @@
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10" t="s">
         <v>4</v>
@@ -10778,7 +10783,7 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:10" ht="15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="32"/>
       <c r="B14" s="5">
         <v>6</v>
       </c>
@@ -10806,7 +10811,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="35" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="9"/>
@@ -10818,7 +10823,7 @@
       <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:10" ht="15">
-      <c r="A16" s="31"/>
+      <c r="A16" s="32"/>
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -10846,7 +10851,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="35" t="s">
         <v>19</v>
       </c>
       <c r="B17" s="9"/>
@@ -10858,7 +10863,7 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:10" ht="30">
-      <c r="A18" s="31"/>
+      <c r="A18" s="32"/>
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -10886,7 +10891,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -10898,7 +10903,7 @@
       <c r="F19" s="8"/>
     </row>
     <row r="20" spans="1:10" ht="30">
-      <c r="A20" s="31"/>
+      <c r="A20" s="32"/>
       <c r="B20" s="5">
         <v>11</v>
       </c>
@@ -10910,7 +10915,7 @@
       <c r="F20" s="8"/>
     </row>
     <row r="21" spans="1:10" ht="15">
-      <c r="A21" s="35"/>
+      <c r="A21" s="36"/>
       <c r="B21" s="5">
         <v>13</v>
       </c>
@@ -10922,7 +10927,7 @@
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="35" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="9"/>
@@ -10934,7 +10939,7 @@
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:10" ht="15">
-      <c r="A23" s="31"/>
+      <c r="A23" s="32"/>
       <c r="B23" s="5">
         <v>14</v>
       </c>
@@ -10962,7 +10967,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="15">
-      <c r="A24" s="31"/>
+      <c r="A24" s="32"/>
       <c r="B24" s="5">
         <v>15</v>
       </c>
@@ -10974,7 +10979,7 @@
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:10" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="35" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="9"/>
@@ -10986,7 +10991,7 @@
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:10" s="1" customFormat="1" ht="30">
-      <c r="A26" s="31"/>
+      <c r="A26" s="32"/>
       <c r="B26" s="23">
         <v>24</v>
       </c>
@@ -11014,7 +11019,7 @@
       </c>
     </row>
     <row r="27" spans="1:10" s="1" customFormat="1" ht="45">
-      <c r="A27" s="31"/>
+      <c r="A27" s="32"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -11026,7 +11031,7 @@
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
-      <c r="A28" s="31"/>
+      <c r="A28" s="32"/>
       <c r="B28" s="9"/>
       <c r="C28" s="10" t="s">
         <v>10</v>
@@ -11036,7 +11041,7 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:10" ht="30">
-      <c r="A29" s="31"/>
+      <c r="A29" s="32"/>
       <c r="B29" s="23">
         <v>26</v>
       </c>
@@ -11064,7 +11069,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="15">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="42" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="9"/>
@@ -11076,7 +11081,7 @@
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:10" ht="15">
-      <c r="A31" s="41"/>
+      <c r="A31" s="42"/>
       <c r="B31" s="5">
         <v>19</v>
       </c>
@@ -11104,7 +11109,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="30">
-      <c r="A32" s="41"/>
+      <c r="A32" s="42"/>
       <c r="B32" s="5">
         <v>20</v>
       </c>
@@ -11116,7 +11121,7 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:10" ht="15">
-      <c r="A33" s="41"/>
+      <c r="A33" s="42"/>
       <c r="B33" s="5">
         <v>21</v>
       </c>
@@ -11128,7 +11133,7 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:10" ht="15">
-      <c r="A34" s="41"/>
+      <c r="A34" s="42"/>
       <c r="B34" s="5">
         <v>24</v>
       </c>
@@ -11140,7 +11145,7 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:10" ht="15">
-      <c r="A35" s="41"/>
+      <c r="A35" s="42"/>
       <c r="B35" s="5">
         <v>25</v>
       </c>
@@ -11152,7 +11157,7 @@
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:10" ht="15" customHeight="1">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="30" t="s">
         <v>30</v>
       </c>
       <c r="B36" s="9"/>
@@ -11164,7 +11169,7 @@
       <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:10" ht="30">
-      <c r="A37" s="30"/>
+      <c r="A37" s="31"/>
       <c r="B37" s="5">
         <v>26</v>
       </c>
@@ -11192,7 +11197,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" ht="15">
-      <c r="A38" s="30"/>
+      <c r="A38" s="31"/>
       <c r="B38" s="5">
         <v>27</v>
       </c>
@@ -11204,7 +11209,7 @@
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:10" ht="30">
-      <c r="A39" s="30"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="5">
         <v>28</v>
       </c>
@@ -11216,7 +11221,7 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:10" ht="15">
-      <c r="A40" s="30"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="5"/>
       <c r="C40" s="8" t="s">
         <v>104</v>
@@ -11226,7 +11231,7 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" spans="1:10" ht="15">
-      <c r="A41" s="30"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="9"/>
       <c r="C41" s="10" t="s">
         <v>15</v>
@@ -11236,7 +11241,7 @@
       <c r="F41" s="12"/>
     </row>
     <row r="42" spans="1:10" ht="15">
-      <c r="A42" s="30"/>
+      <c r="A42" s="31"/>
       <c r="B42" s="5">
         <v>29</v>
       </c>
@@ -11264,7 +11269,7 @@
       </c>
     </row>
     <row r="43" spans="1:10" ht="15">
-      <c r="A43" s="30"/>
+      <c r="A43" s="31"/>
       <c r="B43" s="5">
         <v>30</v>
       </c>
@@ -11305,6 +11310,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11312,11 +11322,6 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
Aplicação do checklist, e alteração no Modelo de Analise e Design em Arquitetura.
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FF876-0099-4A5A-B689-FCE93039BA63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF05012F-E1C3-4868-8353-689FDEA067E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="117">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1053,9 +1053,6 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>Todas as tarefas devem ser lançadas no backlog do produto no github. No sprint ficam apenas as tarefas do sprint puxadas do backlog.</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1385,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1511,6 +1508,12 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1611,18 +1614,18 @@
             <c:numRef>
               <c:f>Indicadores!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.91304347826086951</c:v>
+                  <c:v>0.95652173913043481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1672,7 +1675,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1858,7 +1861,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1971,7 +1974,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2577,37 +2580,37 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2720,7 +2723,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2922,7 +2925,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2940,7 +2943,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
@@ -7300,8 +7303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7328,18 +7331,18 @@
       <c r="A3" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="47">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.91304347826086951</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="20" t="e">
+      <c r="B4" s="47">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7447,21 +7450,21 @@
       <c r="N2" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="25" t="e">
+      <c r="O2" s="25">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P2" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P2" s="25">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="25">
         <f>('Ver-Elaboração1'!$I$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R2" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R2" s="25">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7487,21 +7490,21 @@
       <c r="N3" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="25" t="e">
+      <c r="O3" s="25">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P3" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P3" s="25">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q3" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="25">
         <f>('Ver-Elaboração1'!$I$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R3" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R3" s="25">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7527,21 +7530,21 @@
       <c r="N4" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="25" t="e">
+      <c r="O4" s="25">
         <f>('Ver-Elaboração1'!$G$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P4" s="25" t="e">
+        <v>0.75</v>
+      </c>
+      <c r="P4" s="25">
         <f>('Ver-Elaboração1'!$H$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q4" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="25">
         <f>('Ver-Elaboração1'!$I$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R4" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R4" s="25">
         <f>('Ver-Elaboração1'!$J$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>#DIV/0!</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7567,21 +7570,21 @@
       <c r="N5" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="25" t="e">
+      <c r="O5" s="25">
         <f>('Ver-Elaboração1'!$G$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P5" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P5" s="25">
         <f>('Ver-Elaboração1'!$H$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="25">
         <f>('Ver-Elaboração1'!$I$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R5" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R5" s="25">
         <f>('Ver-Elaboração1'!$J$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7590,11 +7593,11 @@
       </c>
       <c r="B6" s="25">
         <f>('Ver-Iniciação1'!$G$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="25">
         <f>('Ver-Iniciação1'!$H$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="25">
         <f>('Ver-Iniciação1'!$I$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
@@ -7647,21 +7650,21 @@
       <c r="N7" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="25" t="e">
+      <c r="O7" s="25">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P7" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P7" s="25">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="25">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R7" s="25">
         <f>('Ver-Elaboração1'!$J$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -7727,21 +7730,21 @@
       <c r="N9" t="s">
         <v>6</v>
       </c>
-      <c r="O9" s="25" t="e">
+      <c r="O9" s="25">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P9" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P9" s="25">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="25">
         <f>('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R9" s="25">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -7767,21 +7770,21 @@
       <c r="N10" t="s">
         <v>13</v>
       </c>
-      <c r="O10" s="25" t="e">
+      <c r="O10" s="25">
         <f>('Ver-Elaboração1'!$G$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P10" s="25" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="P10" s="25">
         <f>('Ver-Elaboração1'!$H$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="25">
         <f>('Ver-Elaboração1'!$I$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R10" s="25">
         <f>('Ver-Elaboração1'!$J$29/SUM('Ver-Elaboração1'!$G$29:'Ver-Elaboração1'!$J$29))</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -7807,21 +7810,21 @@
       <c r="N11" t="s">
         <v>56</v>
       </c>
-      <c r="O11" s="25" t="e">
+      <c r="O11" s="25">
         <f>('Ver-Elaboração1'!$G$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P11" s="25" t="e">
+        <v>1</v>
+      </c>
+      <c r="P11" s="25">
         <f>('Ver-Elaboração1'!$H$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="25">
         <f>('Ver-Elaboração1'!$I$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R11" s="25">
         <f>('Ver-Elaboração1'!$J$36/SUM('Ver-Elaboração1'!$G$36:'Ver-Elaboração1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -7847,21 +7850,21 @@
       <c r="N12" t="s">
         <v>15</v>
       </c>
-      <c r="O12" s="25" t="e">
+      <c r="O12" s="25">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P12" s="25" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="25">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q12" s="25" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="Q12" s="25">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R12" s="25" t="e">
+        <v>0</v>
+      </c>
+      <c r="R12" s="25">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -8414,8 +8417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8454,7 +8457,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.91304347826086951</v>
+        <v>0.95652173913043481</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -8790,11 +8793,11 @@
       <c r="F22" s="12"/>
       <c r="G22">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <f>COUNTIF(D23:D24,"Não")</f>
@@ -8805,7 +8808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="75">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="32"/>
       <c r="B23" s="23">
         <v>14</v>
@@ -8814,11 +8817,9 @@
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>117</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15">
@@ -9137,8 +9138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9172,9 +9173,9 @@
         <v>44</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="21" t="e">
+      <c r="F2" s="46">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9229,12 +9230,14 @@
       <c r="C6" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -9267,12 +9270,14 @@
       <c r="C8" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -9295,7 +9300,9 @@
       <c r="C9" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
       <c r="G9"/>
@@ -9321,12 +9328,14 @@
       <c r="C11" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
       <c r="G11">
         <f>COUNTIF(D11:D14,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H11">
         <f>COUNTIF(D11:D14,"Parcialmente")</f>
@@ -9338,7 +9347,7 @@
       </c>
       <c r="J11">
         <f>COUNTIF(D11:D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
@@ -9349,7 +9358,9 @@
       <c r="C12" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -9361,7 +9372,9 @@
       <c r="C13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
@@ -9373,7 +9386,9 @@
       <c r="C14" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
@@ -9395,12 +9410,14 @@
       <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -9435,12 +9452,14 @@
       <c r="C18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
@@ -9463,7 +9482,9 @@
       <c r="C19" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -9475,7 +9496,9 @@
       <c r="C20" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -9487,7 +9510,9 @@
       <c r="C21" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -9511,12 +9536,14 @@
       <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
@@ -9539,7 +9566,9 @@
       <c r="C24" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -9551,7 +9580,9 @@
       <c r="C25" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
@@ -9563,7 +9594,9 @@
       <c r="C26" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -9575,7 +9608,9 @@
       <c r="C27" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -9599,12 +9634,14 @@
       <c r="C29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29">
         <f>COUNTIF(D29:D34,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H29">
         <f>COUNTIF(D29:D34,"Parcialmente")</f>
@@ -9616,7 +9653,7 @@
       </c>
       <c r="J29">
         <f>COUNTIF(D29:D34,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15">
@@ -9627,7 +9664,9 @@
       <c r="C30" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
@@ -9639,7 +9678,9 @@
       <c r="C31" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -9651,7 +9692,9 @@
       <c r="C32" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
@@ -9663,7 +9706,9 @@
       <c r="C33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -9675,7 +9720,9 @@
       <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -9699,12 +9746,14 @@
       <c r="C36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
@@ -9727,7 +9776,9 @@
       <c r="C37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -9739,7 +9790,9 @@
       <c r="C38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -9761,16 +9814,18 @@
       <c r="C40" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40">
         <f>COUNTIF(D40:D41,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <f>COUNTIF(D40:D41,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <f>COUNTIF(D40:D41,"Não")</f>
@@ -9789,7 +9844,9 @@
       <c r="C41" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
@@ -10531,17 +10588,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0400-000000000000}">
@@ -11310,11 +11367,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11322,6 +11374,11 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0500-000000000000}">

</xml_diff>

<commit_message>
alterações nos documentos de gerenciamento
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF05012F-E1C3-4868-8353-689FDEA067E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA9DBE-1551-4A28-95BF-0F8FFDF1CA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1053,6 +1053,24 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Deve ser app web</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Uma histpria por caso de uso. A tabela de casos de teste deve testar apenas o caso de uso corrente.</t>
+  </si>
+  <si>
+    <t>Todas as tarefas devem ser lançadas no backlog do produto no github. No sprint ficam apenas as tarefas do sprint puxadas do backlog.</t>
+  </si>
+  <si>
+    <t>não há indicação de qual padrão de codificação foi utilizado</t>
+  </si>
+  <si>
+    <t>Não há evidencias</t>
   </si>
 </sst>
 </file>
@@ -1385,7 +1403,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1508,12 +1526,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1614,18 +1626,18 @@
             <c:numRef>
               <c:f>Indicadores!$B$3:$B$6</c:f>
               <c:numCache>
-                <c:formatCode>0%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.95652173913043481</c:v>
+                  <c:v>0.82608695652173914</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.96</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
+                  <c:v>0.80952380952380953</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1675,7 +1687,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1852,16 +1864,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1965,7 +1977,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1974,7 +1986,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2084,7 +2096,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2580,28 +2592,28 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>0.75</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.66666666666666663</c:v>
@@ -2610,7 +2622,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2714,7 +2726,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2723,7 +2735,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2821,13 +2833,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2919,16 +2931,16 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2949,7 +2961,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3310,10 +3322,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3334,7 +3346,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -3432,7 +3444,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -3664,22 +3676,22 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -7303,8 +7315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7331,27 +7343,27 @@
       <c r="A3" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="47">
+      <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.95652173913043481</v>
+        <v>0.82608695652173914</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="47">
+      <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.96</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="20" t="e">
+      <c r="B5" s="20">
         <f>'Ver-Construção1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7452,7 +7464,7 @@
       </c>
       <c r="O2" s="25">
         <f>('Ver-Elaboração1'!$G$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2" s="25">
         <f>('Ver-Elaboração1'!$H$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
@@ -7464,7 +7476,7 @@
       </c>
       <c r="R2" s="25">
         <f>('Ver-Elaboração1'!$J$6/SUM('Ver-Elaboração1'!$G$6:'Ver-Elaboração1'!$J$6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -7473,11 +7485,11 @@
       </c>
       <c r="B3" s="25">
         <f>('Ver-Iniciação1'!$G$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C3" s="25">
         <f>('Ver-Iniciação1'!$H$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="D3" s="25">
         <f>('Ver-Iniciação1'!$I$7/SUM('Ver-Iniciação1'!$G$7:'Ver-Iniciação1'!$J$7))</f>
@@ -7492,7 +7504,7 @@
       </c>
       <c r="O3" s="25">
         <f>('Ver-Elaboração1'!$G$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="25">
         <f>('Ver-Elaboração1'!$H$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
@@ -7504,7 +7516,7 @@
       </c>
       <c r="R3" s="25">
         <f>('Ver-Elaboração1'!$J$8/SUM('Ver-Elaboração1'!$G$8:'Ver-Elaboração1'!$J$8))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -7532,7 +7544,7 @@
       </c>
       <c r="O4" s="25">
         <f>('Ver-Elaboração1'!$G$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="P4" s="25">
         <f>('Ver-Elaboração1'!$H$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
@@ -7544,7 +7556,7 @@
       </c>
       <c r="R4" s="25">
         <f>('Ver-Elaboração1'!$J$11/SUM('Ver-Elaboração1'!$G$11:'Ver-Elaboração1'!$J$11))</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:18">
@@ -7553,7 +7565,7 @@
       </c>
       <c r="B5" s="25">
         <f>('Ver-Iniciação1'!$G$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C5" s="25">
         <f>('Ver-Iniciação1'!$H$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
@@ -7561,7 +7573,7 @@
       </c>
       <c r="D5" s="25">
         <f>('Ver-Iniciação1'!$I$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E5" s="25">
         <f>('Ver-Iniciação1'!$J$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
@@ -7572,7 +7584,7 @@
       </c>
       <c r="O5" s="25">
         <f>('Ver-Elaboração1'!$G$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="25">
         <f>('Ver-Elaboração1'!$H$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
@@ -7584,7 +7596,7 @@
       </c>
       <c r="R5" s="25">
         <f>('Ver-Elaboração1'!$J$16/SUM('Ver-Elaboração1'!$G$16:'Ver-Elaboração1'!$J$16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -7593,11 +7605,11 @@
       </c>
       <c r="B6" s="25">
         <f>('Ver-Iniciação1'!$G$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C6" s="25">
         <f>('Ver-Iniciação1'!$H$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D6" s="25">
         <f>('Ver-Iniciação1'!$I$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
@@ -7652,7 +7664,7 @@
       </c>
       <c r="O7" s="25">
         <f>('Ver-Elaboração1'!$G$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="P7" s="25">
         <f>('Ver-Elaboração1'!$H$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
@@ -7660,7 +7672,7 @@
       </c>
       <c r="Q7" s="25">
         <f>('Ver-Elaboração1'!$I$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="R7" s="25">
         <f>('Ver-Elaboração1'!$J$18/SUM('Ver-Elaboração1'!$G$18:'Ver-Elaboração1'!$J$18))</f>
@@ -7732,15 +7744,15 @@
       </c>
       <c r="O9" s="25">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="P9" s="25">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Q9" s="25">
         <f>('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="R9" s="25">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
@@ -7852,11 +7864,11 @@
       </c>
       <c r="O12" s="25">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="P12" s="25">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="25">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
@@ -7864,7 +7876,7 @@
       </c>
       <c r="R12" s="25">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -7888,42 +7900,42 @@
       <c r="A23" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="26" t="e">
+      <c r="B23" s="26">
         <f>('Ver-Construção1'!$G$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C23" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="C23" s="27">
         <f>('Ver-Construção1'!$H$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D23" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D23" s="27">
         <f>('Ver-Construção1'!$I$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E23" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E23" s="27">
         <f>('Ver-Construção1'!$J$6/SUM('Ver-Construção1'!$G$6:'Ver-Construção1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:17">
       <c r="A24" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="26" t="e">
+      <c r="B24" s="26">
         <f>('Ver-Construção1'!$G$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C24" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="C24" s="27">
         <f>('Ver-Construção1'!$H$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D24" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D24" s="27">
         <f>('Ver-Construção1'!$I$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E24" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E24" s="27">
         <f>('Ver-Construção1'!$J$8/SUM('Ver-Construção1'!$G$8:'Ver-Construção1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M24" t="s">
         <v>91</v>
@@ -7945,21 +7957,21 @@
       <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="26" t="e">
+      <c r="B25" s="26">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C25" s="27" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C25" s="27">
         <f>('Ver-Construção1'!$G$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D25" s="27" t="e">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D25" s="27">
         <f>('Ver-Construção1'!$I$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E25" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E25" s="27">
         <f>('Ver-Construção1'!$J$10/SUM('Ver-Construção1'!$G$10:'Ver-Construção1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="M25" t="s">
         <v>2</v>
@@ -7985,21 +7997,21 @@
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="27" t="e">
+      <c r="B26" s="27">
         <f>('Ver-Construção1'!$G$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C26" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="C26" s="27">
         <f>('Ver-Construção1'!$H$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D26" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
         <f>('Ver-Construção1'!$I$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E26" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E26" s="27">
         <f>('Ver-Construção1'!$J$14/SUM('Ver-Construção1'!$G$14:'Ver-Construção1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M26" t="s">
         <v>3</v>
@@ -8065,21 +8077,21 @@
       <c r="A28" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="27" t="e">
+      <c r="B28" s="27">
         <f>('Ver-Construção1'!$G$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="C28" s="27">
         <f>('Ver-Construção1'!$H$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D28" s="27">
         <f>('Ver-Construção1'!$I$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E28" s="27">
         <f>('Ver-Construção1'!$J$16/SUM('Ver-Construção1'!$G$16:'Ver-Construção1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="M28" t="s">
         <v>4</v>
@@ -8225,21 +8237,21 @@
       <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="27" t="e">
+      <c r="B32" s="27">
         <f>('Ver-Construção1'!$G$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C32" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="C32" s="27">
         <f>('Ver-Construção1'!$H$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D32" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D32" s="27">
         <f>('Ver-Construção1'!$I$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E32" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E32" s="27">
         <f>('Ver-Construção1'!$J$30/SUM('Ver-Construção1'!$G$30:'Ver-Construção1'!$J$30))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M32" t="s">
         <v>8</v>
@@ -8417,8 +8429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8457,7 +8469,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.95652173913043481</v>
+        <v>0.82608695652173914</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -8547,11 +8559,11 @@
       <c r="F7" s="12"/>
       <c r="G7">
         <f>COUNTIF(D8:D12,"Sim")</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H7">
         <f>COUNTIF(D8:D12,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <f>COUNTIF(D8:D12,"Não")</f>
@@ -8627,9 +8639,11 @@
         <v>40</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E12" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>117</v>
+      </c>
       <c r="F12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="15">
@@ -8739,7 +8753,7 @@
       <c r="F19" s="12"/>
       <c r="G19">
         <f>COUNTIF(D20:D21,"Sim")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D20:D21,"Parcialmente")</f>
@@ -8747,7 +8761,7 @@
       </c>
       <c r="I19">
         <f>COUNTIF(D20:D21,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <f>COUNTIF(D20:D21,"NA")</f>
@@ -8768,7 +8782,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="30">
+    <row r="21" spans="1:10" ht="60">
       <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>13</v>
@@ -8777,9 +8791,11 @@
         <v>115</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="8"/>
+        <v>118</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>119</v>
+      </c>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
@@ -8793,11 +8809,11 @@
       <c r="F22" s="12"/>
       <c r="G22">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <f>COUNTIF(D23:D24,"Não")</f>
@@ -8808,7 +8824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15">
+    <row r="23" spans="1:10" ht="75">
       <c r="A23" s="32"/>
       <c r="B23" s="23">
         <v>14</v>
@@ -8817,9 +8833,11 @@
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>120</v>
+      </c>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15">
@@ -9124,7 +9142,7 @@
     <mergeCell ref="D2:E2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{D862B195-455A-4EFD-824E-16CDF79502AC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D20:D21 D23:D24 D26:D27 D38:D41 D14:D18 D8:D12 D29:D36" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9138,8 +9156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9173,9 +9191,9 @@
         <v>44</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="46">
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.96</v>
+        <v>0.80952380952380953</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9231,13 +9249,13 @@
         <v>107</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
         <f>COUNTIF(D6,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>COUNTIF(D6,"Parcialmente")</f>
@@ -9249,7 +9267,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
@@ -9271,13 +9289,13 @@
         <v>108</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -9289,7 +9307,7 @@
       </c>
       <c r="J8">
         <f>COUNTIF(D8,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="1" customFormat="1" ht="30">
@@ -9335,7 +9353,7 @@
       <c r="F11" s="8"/>
       <c r="G11">
         <f>COUNTIF(D11:D14,"Sim")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H11">
         <f>COUNTIF(D11:D14,"Parcialmente")</f>
@@ -9347,7 +9365,7 @@
       </c>
       <c r="J11">
         <f>COUNTIF(D11:D14,"NA")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30">
@@ -9373,7 +9391,7 @@
         <v>45</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -9411,13 +9429,13 @@
         <v>46</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
         <f>COUNTIF(D16,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16">
         <f>COUNTIF(D16,"Parcialmente")</f>
@@ -9429,7 +9447,7 @@
       </c>
       <c r="J16">
         <f>COUNTIF(D16,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
@@ -9459,7 +9477,7 @@
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
@@ -9467,7 +9485,7 @@
       </c>
       <c r="I18">
         <f>COUNTIF(D18:D21,"Não")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J18">
         <f>COUNTIF(D18:D21,"NA")</f>
@@ -9497,7 +9515,7 @@
         <v>61</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -9543,15 +9561,15 @@
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <f>COUNTIF(D23:D27,"Não")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23">
         <f>COUNTIF(D23:D27,"NA")</f>
@@ -9572,7 +9590,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:10" ht="30">
+    <row r="25" spans="1:10" ht="45">
       <c r="A25" s="32"/>
       <c r="B25" s="5">
         <v>19</v>
@@ -9581,9 +9599,11 @@
         <v>98</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="8"/>
+        <v>114</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="F25" s="8"/>
     </row>
     <row r="26" spans="1:10" ht="15">
@@ -9595,7 +9615,7 @@
         <v>99</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -9609,9 +9629,11 @@
         <v>100</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="8"/>
+        <v>118</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>122</v>
+      </c>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
@@ -9679,7 +9701,7 @@
         <v>52</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
@@ -9693,7 +9715,7 @@
         <v>87</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
@@ -9815,17 +9837,17 @@
         <v>105</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40">
         <f>COUNTIF(D40:D41,"Sim")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H40">
         <f>COUNTIF(D40:D41,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <f>COUNTIF(D40:D41,"Não")</f>
@@ -9833,7 +9855,7 @@
       </c>
       <c r="J40">
         <f>COUNTIF(D40:D41,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15">
@@ -9845,7 +9867,7 @@
         <v>106</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -9880,8 +9902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9915,9 +9937,9 @@
         <v>44</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="21" t="e">
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D42,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9972,7 +9994,9 @@
       <c r="C6" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
@@ -9989,7 +10013,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
@@ -10010,12 +10034,14 @@
       <c r="C8" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -10048,12 +10074,14 @@
       <c r="C10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -10065,7 +10093,7 @@
       </c>
       <c r="J10">
         <f>COUNTIF(D10:D12,"NA")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
@@ -10076,7 +10104,9 @@
       <c r="C11" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -10088,7 +10118,9 @@
       <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -10110,7 +10142,9 @@
       <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14">
@@ -10127,7 +10161,7 @@
       </c>
       <c r="J14">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
@@ -10150,7 +10184,9 @@
       <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
@@ -10167,7 +10203,7 @@
       </c>
       <c r="J16">
         <f>COUNTIF(D16:D16,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15">
@@ -10366,12 +10402,14 @@
       <c r="C30" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
       <c r="G30">
         <f>COUNTIF(D30:D34,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H30">
         <f>COUNTIF(D30:D34,"Parcialmente")</f>
@@ -10394,7 +10432,9 @@
       <c r="C31" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
@@ -10406,7 +10446,9 @@
       <c r="C32" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>

</xml_diff>

<commit_message>
atualização no diagrama e checklist
</commit_message>
<xml_diff>
--- a/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
+++ b/CHP/6.Gerenciamento de Projeto/CHP - Checklist Verificacao de Projeto.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFA9DBE-1551-4A28-95BF-0F8FFDF1CA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591386B1-6341-475A-B8D7-19B1B2F23A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="666" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indicadores" sheetId="6" r:id="rId1"/>
@@ -702,7 +702,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="120">
   <si>
     <t>Ambiente</t>
   </si>
@@ -1061,16 +1061,7 @@
     <t>Não</t>
   </si>
   <si>
-    <t>Uma histpria por caso de uso. A tabela de casos de teste deve testar apenas o caso de uso corrente.</t>
-  </si>
-  <si>
-    <t>Todas as tarefas devem ser lançadas no backlog do produto no github. No sprint ficam apenas as tarefas do sprint puxadas do backlog.</t>
-  </si>
-  <si>
     <t>não há indicação de qual padrão de codificação foi utilizado</t>
-  </si>
-  <si>
-    <t>Não há evidencias</t>
   </si>
 </sst>
 </file>
@@ -1629,16 +1620,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.82608695652173914</c:v>
+                  <c:v>0.91304347826086951</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80952380952380953</c:v>
+                  <c:v>0.86956521739130432</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.86363636363636365</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1870,10 +1861,10 @@
                   <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1986,7 +1977,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -2096,7 +2087,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2613,7 +2604,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.66666666666666663</c:v>
@@ -2622,7 +2613,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2735,7 +2726,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2839,7 +2830,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2961,7 +2952,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3340,19 +3331,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3471,7 +3462,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4073,10 +4064,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -4088,25 +4079,25 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4219,10 +4210,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -4231,7 +4222,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4445,22 +4436,22 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -4475,7 +4466,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -7345,7 +7336,7 @@
       </c>
       <c r="B3" s="20">
         <f>'Ver-Iniciação1'!$F$2</f>
-        <v>0.82608695652173914</v>
+        <v>0.91304347826086951</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7354,7 +7345,7 @@
       </c>
       <c r="B4" s="20">
         <f>'Ver-Elaboração1'!$F$2</f>
-        <v>0.80952380952380953</v>
+        <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -7370,9 +7361,9 @@
       <c r="A6" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="20" t="e">
+      <c r="B6" s="20">
         <f>'Ver-Transição1'!$F$2</f>
-        <v>#DIV/0!</v>
+        <v>0.86363636363636365</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -7391,7 +7382,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="AA36" sqref="AA36"/>
     </sheetView>
   </sheetViews>
@@ -7565,7 +7556,7 @@
       </c>
       <c r="B5" s="25">
         <f>('Ver-Iniciação1'!$G$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5" s="25">
         <f>('Ver-Iniciação1'!$H$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
@@ -7573,7 +7564,7 @@
       </c>
       <c r="D5" s="25">
         <f>('Ver-Iniciação1'!$I$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="25">
         <f>('Ver-Iniciação1'!$J$19/SUM('Ver-Iniciação1'!$G$19:'Ver-Iniciação1'!$J$19))</f>
@@ -7605,11 +7596,11 @@
       </c>
       <c r="B6" s="25">
         <f>('Ver-Iniciação1'!$G$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="25">
         <f>('Ver-Iniciação1'!$H$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6" s="25">
         <f>('Ver-Iniciação1'!$I$22/SUM('Ver-Iniciação1'!$G$22:'Ver-Iniciação1'!$J$22))</f>
@@ -7744,7 +7735,7 @@
       </c>
       <c r="O9" s="25">
         <f>('Ver-Elaboração1'!$G$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="P9" s="25">
         <f>('Ver-Elaboração1'!$H$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
@@ -7752,7 +7743,7 @@
       </c>
       <c r="Q9" s="25">
         <f>('Ver-Elaboração1'!$I$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="R9" s="25">
         <f>('Ver-Elaboração1'!$J$23/SUM('Ver-Elaboração1'!$G$23:'Ver-Elaboração1'!$J$23))</f>
@@ -7864,11 +7855,11 @@
       </c>
       <c r="O12" s="25">
         <f>('Ver-Elaboração1'!$G$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P12" s="25">
         <f>('Ver-Elaboração1'!$H$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q12" s="25">
         <f>('Ver-Elaboração1'!$I$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
@@ -7876,7 +7867,7 @@
       </c>
       <c r="R12" s="25">
         <f>('Ver-Elaboração1'!$J$40/SUM('Ver-Elaboração1'!$G$40:'Ver-Elaboração1'!$J$40))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -7976,21 +7967,21 @@
       <c r="M25" t="s">
         <v>2</v>
       </c>
-      <c r="N25" s="27" t="e">
+      <c r="N25" s="27">
         <f>('Ver-Transição1'!$G$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="O25" s="27">
         <f>('Ver-Transição1'!$H$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P25" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P25" s="27">
         <f>('Ver-Transição1'!$I$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q25" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="27">
         <f>('Ver-Transição1'!$J$6/SUM('Ver-Transição1'!$G$6:'Ver-Transição1'!$J$6))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -8016,21 +8007,21 @@
       <c r="M26" t="s">
         <v>3</v>
       </c>
-      <c r="N26" s="27" t="e">
+      <c r="N26" s="27">
         <f>('Ver-Transição1'!$G$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="O26" s="27">
         <f>('Ver-Transição1'!$H$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P26" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P26" s="27">
         <f>('Ver-Transição1'!$I$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q26" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="27">
         <f>('Ver-Transição1'!$J$8/SUM('Ver-Transição1'!$G$8:'Ver-Transição1'!$J$8))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -8056,21 +8047,21 @@
       <c r="M27" t="s">
         <v>14</v>
       </c>
-      <c r="N27" s="27" t="e">
+      <c r="N27" s="27">
         <f>('Ver-Transição1'!$G$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" s="27" t="e">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="O27" s="27">
         <f>('Ver-Transição1'!$H$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P27" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P27" s="27">
         <f>('Ver-Transição1'!$I$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q27" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="27">
         <f>('Ver-Transição1'!$J$10/SUM('Ver-Transição1'!$G$10:'Ver-Transição1'!$J$10))</f>
-        <v>#DIV/0!</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -8096,21 +8087,21 @@
       <c r="M28" t="s">
         <v>4</v>
       </c>
-      <c r="N28" s="27" t="e">
+      <c r="N28" s="27">
         <f>('Ver-Transição1'!$G$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="O28" s="27">
         <f>('Ver-Transição1'!$H$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P28" s="27">
         <f>('Ver-Transição1'!$I$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q28" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="27">
         <f>('Ver-Transição1'!$J$14/SUM('Ver-Transição1'!$G$14:'Ver-Transição1'!$J$14))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -8157,80 +8148,80 @@
       <c r="A30" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="27" t="e">
+      <c r="B30" s="27">
         <f>('Ver-Construção1'!$G$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C30" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="C30" s="27">
         <f>('Ver-Construção1'!$H$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D30" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D30" s="27">
         <f>('Ver-Construção1'!$I$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E30" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E30" s="27">
         <f>('Ver-Construção1'!$J$18/SUM('Ver-Construção1'!$G$18:'Ver-Construção1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M30" t="s">
         <v>5</v>
       </c>
-      <c r="N30" s="27" t="e">
+      <c r="N30" s="27">
         <f>('Ver-Transição1'!$G$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O30" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="O30" s="27">
         <f>('Ver-Transição1'!$H$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P30" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P30" s="27">
         <f>('Ver-Transição1'!$I$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q30" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="27">
         <f>('Ver-Transição1'!$J$16/SUM('Ver-Transição1'!$G$16:'Ver-Transição1'!$J$16))</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:17">
       <c r="A31" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="27" t="e">
+      <c r="B31" s="27">
         <f>('Ver-Construção1'!$G$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C31" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="C31" s="27">
         <f>('Ver-Construção1'!$H$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D31" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D31" s="27">
         <f>('Ver-Construção1'!$I$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E31" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E31" s="27">
         <f>('Ver-Construção1'!$J$24/SUM('Ver-Construção1'!$G$24:'Ver-Construção1'!$J$24))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M31" t="s">
         <v>6</v>
       </c>
-      <c r="N31" s="27" t="e">
+      <c r="N31" s="27">
         <f>('Ver-Transição1'!$G$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="O31" s="27">
         <f>('Ver-Transição1'!$H$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P31" s="27">
         <f>('Ver-Transição1'!$I$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q31" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="27">
         <f>('Ver-Transição1'!$J$18/SUM('Ver-Transição1'!$G$18:'Ver-Transição1'!$J$18))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -8256,164 +8247,164 @@
       <c r="M32" t="s">
         <v>8</v>
       </c>
-      <c r="N32" s="27" t="e">
+      <c r="N32" s="27">
         <f>('Ver-Transição1'!$G$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O32" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="O32" s="27">
         <f>('Ver-Transição1'!$H$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P32" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P32" s="27">
         <f>('Ver-Transição1'!$I$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q32" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="27">
         <f>('Ver-Transição1'!$J$23/SUM('Ver-Transição1'!$G$23:'Ver-Transição1'!$J$23))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:17">
       <c r="A33" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="27" t="e">
+      <c r="B33" s="27">
         <f>('Ver-Construção1'!$G$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C33" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="C33" s="27">
         <f>('Ver-Construção1'!$H$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D33" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="D33" s="27">
         <f>('Ver-Construção1'!$I$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E33" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E33" s="27">
         <f>('Ver-Construção1'!$J$36/SUM('Ver-Construção1'!$G$36:'Ver-Construção1'!$J$36))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M33" t="s">
         <v>9</v>
       </c>
-      <c r="N33" s="27" t="e">
+      <c r="N33" s="27">
         <f>('Ver-Transição1'!$G$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O33" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="O33" s="27">
         <f>('Ver-Transição1'!$H$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P33" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="P33" s="27">
         <f>('Ver-Transição1'!$I$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q33" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="27">
         <f>('Ver-Transição1'!$J$26/SUM('Ver-Transição1'!$G$26:'Ver-Transição1'!$J$26))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:17">
       <c r="A34" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="27" t="e">
+      <c r="B34" s="27">
         <f>('Ver-Construção1'!$G$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C34" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="C34" s="27">
         <f>('Ver-Construção1'!$H$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D34" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="D34" s="27">
         <f>('Ver-Construção1'!$I$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E34" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="E34" s="27">
         <f>('Ver-Construção1'!$J$41/SUM('Ver-Construção1'!$G$41:'Ver-Construção1'!$J$41))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="M34" t="s">
         <v>10</v>
       </c>
-      <c r="N34" s="26" t="e">
+      <c r="N34" s="26">
         <f>('Ver-Transição1'!$G$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O34" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="O34" s="27">
         <f>('Ver-Transição1'!$H$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P34" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="P34" s="27">
         <f>('Ver-Transição1'!$I$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q34" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="27">
         <f>('Ver-Transição1'!$J$29/SUM('Ver-Transição1'!$G$29:'Ver-Transição1'!$J$29))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:17">
       <c r="M35" t="s">
         <v>13</v>
       </c>
-      <c r="N35" s="27" t="e">
+      <c r="N35" s="27">
         <f>('Ver-Transição1'!$G$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O35" s="27" t="e">
+        <v>0.8</v>
+      </c>
+      <c r="O35" s="27">
         <f>('Ver-Transição1'!$H$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P35" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P35" s="27">
         <f>('Ver-Transição1'!$I$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q35" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="27">
         <f>('Ver-Transição1'!$J$31/SUM('Ver-Transição1'!$G$31:'Ver-Transição1'!$J$31))</f>
-        <v>#DIV/0!</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:17">
       <c r="M36" t="s">
         <v>56</v>
       </c>
-      <c r="N36" s="27" t="e">
+      <c r="N36" s="27">
         <f>('Ver-Transição1'!$G$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O36" s="27" t="e">
+        <v>1</v>
+      </c>
+      <c r="O36" s="27">
         <f>('Ver-Transição1'!$H$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P36" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="P36" s="27">
         <f>('Ver-Transição1'!$I$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q36" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="27">
         <f>('Ver-Transição1'!$J$37/SUM('Ver-Transição1'!$G$37:'Ver-Transição1'!$J$37))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:17">
       <c r="M37" t="s">
         <v>15</v>
       </c>
-      <c r="N37" s="27" t="e">
+      <c r="N37" s="27">
         <f>('Ver-Transição1'!$G$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O37" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="O37" s="27">
         <f>('Ver-Transição1'!$H$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P37" s="27" t="e">
+        <v>0.5</v>
+      </c>
+      <c r="P37" s="27">
         <f>('Ver-Transição1'!$I$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q37" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="27">
         <f>('Ver-Transição1'!$J$42/SUM('Ver-Transição1'!$G$42:'Ver-Transição1'!$J$42))</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8429,8 +8420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="B16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -8469,7 +8460,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D41)-COUNTIF(D5:D41,"NA"))</f>
-        <v>0.82608695652173914</v>
+        <v>0.91304347826086951</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -8753,7 +8744,7 @@
       <c r="F19" s="12"/>
       <c r="G19">
         <f>COUNTIF(D20:D21,"Sim")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <f>COUNTIF(D20:D21,"Parcialmente")</f>
@@ -8761,7 +8752,7 @@
       </c>
       <c r="I19">
         <f>COUNTIF(D20:D21,"Não")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f>COUNTIF(D20:D21,"NA")</f>
@@ -8782,7 +8773,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:10" ht="60">
+    <row r="21" spans="1:10" ht="30">
       <c r="A21" s="32"/>
       <c r="B21" s="5">
         <v>13</v>
@@ -8791,11 +8782,9 @@
         <v>115</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>119</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
     <row r="22" spans="1:10" ht="15">
@@ -8809,11 +8798,11 @@
       <c r="F22" s="12"/>
       <c r="G22">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H22">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <f>COUNTIF(D23:D24,"Não")</f>
@@ -8824,7 +8813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="75">
+    <row r="23" spans="1:10" ht="15">
       <c r="A23" s="32"/>
       <c r="B23" s="23">
         <v>14</v>
@@ -8833,11 +8822,9 @@
         <v>72</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>120</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
     <row r="24" spans="1:10" ht="15">
@@ -9156,8 +9143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -9193,7 +9180,7 @@
       <c r="E2" s="41"/>
       <c r="F2" s="21">
         <f>COUNTIF(D5:D41,"Sim")/(COUNTA(D5:D42)-COUNTIF(D5:D42,"NA"))</f>
-        <v>0.80952380952380953</v>
+        <v>0.86956521739130432</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -9561,7 +9548,7 @@
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D27,"Sim")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D27,"Parcialmente")</f>
@@ -9569,7 +9556,7 @@
       </c>
       <c r="I23">
         <f>COUNTIF(D23:D27,"Não")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <f>COUNTIF(D23:D27,"NA")</f>
@@ -9602,7 +9589,7 @@
         <v>114</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" s="8"/>
     </row>
@@ -9615,7 +9602,7 @@
         <v>99</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -9629,11 +9616,9 @@
         <v>100</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>122</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
     <row r="28" spans="1:10" ht="15">
@@ -9837,17 +9822,17 @@
         <v>105</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40">
         <f>COUNTIF(D40:D41,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <f>COUNTIF(D40:D41,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <f>COUNTIF(D40:D41,"Não")</f>
@@ -9855,7 +9840,7 @@
       </c>
       <c r="J40">
         <f>COUNTIF(D40:D41,"NA")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="15">
@@ -9867,7 +9852,7 @@
         <v>106</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
@@ -9902,8 +9887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10226,12 +10211,14 @@
       <c r="C18" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D22,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D22,"Parcialmente")</f>
@@ -10254,7 +10241,9 @@
       <c r="C19" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -10266,7 +10255,9 @@
       <c r="C20" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -10278,7 +10269,9 @@
       <c r="C21" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -10290,7 +10283,9 @@
       <c r="C22" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
@@ -10314,12 +10309,14 @@
       <c r="C24" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
       <c r="G24">
         <f>COUNTIF(D24:D28,"Sim")</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <f>COUNTIF(D24:D28,"Parcialmente")</f>
@@ -10342,7 +10339,9 @@
       <c r="C25" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
@@ -10354,7 +10353,9 @@
       <c r="C26" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
@@ -10366,7 +10367,9 @@
       <c r="C27" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -10378,7 +10381,9 @@
       <c r="C28" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
@@ -10409,7 +10414,7 @@
       <c r="F30" s="8"/>
       <c r="G30">
         <f>COUNTIF(D30:D34,"Sim")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H30">
         <f>COUNTIF(D30:D34,"Parcialmente")</f>
@@ -10460,7 +10465,9 @@
       <c r="C33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -10472,7 +10479,9 @@
       <c r="C34" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -10496,12 +10505,14 @@
       <c r="C36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36">
         <f>COUNTIF(D36:D38,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H36">
         <f>COUNTIF(D36:D38,"Parcialmente")</f>
@@ -10524,7 +10535,9 @@
       <c r="C37" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
@@ -10536,7 +10549,9 @@
       <c r="C38" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -10546,7 +10561,9 @@
       <c r="C39" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -10568,16 +10585,18 @@
       <c r="C41" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41">
         <f>COUNTIF(D41:D42,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <f>COUNTIF(D41:D42,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <f>COUNTIF(D41:D42,"Não")</f>
@@ -10596,7 +10615,9 @@
       <c r="C42" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
@@ -10630,23 +10651,23 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:F3"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A17:A22"/>
     <mergeCell ref="A29:A34"/>
     <mergeCell ref="A35:A42"/>
     <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:F3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D23 D15 D17 D40 D35 D29" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D36:D39 D41:D42 D18:D22 D24:D28 D30:D34" xr:uid="{00000000-0002-0000-0400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D30:D34 D36:D39 D24:D28 D18:D22 D41:D42" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10659,8 +10680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -10694,9 +10715,9 @@
         <v>44</v>
       </c>
       <c r="E2" s="41"/>
-      <c r="F2" s="21" t="e">
+      <c r="F2" s="21">
         <f>COUNTIF(D5:D43,"Sim")/(COUNTA(D5:D43)-COUNTIF(D5:D43,"NA"))</f>
-        <v>#DIV/0!</v>
+        <v>0.86363636363636365</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" thickBot="1">
@@ -10751,7 +10772,9 @@
       <c r="C6" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6">
@@ -10768,7 +10791,7 @@
       </c>
       <c r="J6">
         <f>COUNTIF(D6,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15">
@@ -10789,12 +10812,14 @@
       <c r="C8" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8">
         <f>COUNTIF(D8,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <f>COUNTIF(D8,"Parcialmente")</f>
@@ -10827,12 +10852,14 @@
       <c r="C10" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10">
         <f>COUNTIF(D10:D12,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H10">
         <f>COUNTIF(D10:D12,"Parcialmente")</f>
@@ -10844,7 +10871,7 @@
       </c>
       <c r="J10">
         <f>COUNTIF(D10:D12,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30">
@@ -10855,7 +10882,9 @@
       <c r="C11" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
@@ -10867,7 +10896,9 @@
       <c r="C12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
@@ -10889,7 +10920,9 @@
       <c r="C14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
       <c r="G14">
@@ -10906,7 +10939,7 @@
       </c>
       <c r="J14">
         <f>COUNTIF(D14,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1">
@@ -10929,7 +10962,9 @@
       <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16">
@@ -10946,7 +10981,7 @@
       </c>
       <c r="J16">
         <f>COUNTIF(D16,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1">
@@ -10969,12 +11004,14 @@
       <c r="C18" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18">
         <f>COUNTIF(D18:D21,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <f>COUNTIF(D18:D21,"Parcialmente")</f>
@@ -10997,7 +11034,9 @@
       <c r="C19" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
@@ -11009,7 +11048,9 @@
       <c r="C20" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
@@ -11021,7 +11062,9 @@
       <c r="C21" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
@@ -11045,12 +11088,14 @@
       <c r="C23" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
       <c r="G23">
         <f>COUNTIF(D23:D24,"Sim")</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23">
         <f>COUNTIF(D23:D24,"Parcialmente")</f>
@@ -11073,7 +11118,9 @@
       <c r="C24" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
@@ -11097,16 +11144,18 @@
       <c r="C26" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
       <c r="G26">
         <f>COUNTIF(D26:D27,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <f>COUNTIF(D26:D27,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <f>COUNTIF(D26:D27,"Não")</f>
@@ -11125,7 +11174,9 @@
       <c r="C27" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
@@ -11147,7 +11198,9 @@
       <c r="C29" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
       <c r="G29">
@@ -11156,7 +11209,7 @@
       </c>
       <c r="H29">
         <f>COUNTIF(D29:D29,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <f>COUNTIF(D29:D29,"Não")</f>
@@ -11187,12 +11240,14 @@
       <c r="C31" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
       <c r="G31">
         <f>COUNTIF(D31:D35,"Sim")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H31">
         <f>COUNTIF(D31:D35,"Parcialmente")</f>
@@ -11204,7 +11259,7 @@
       </c>
       <c r="J31">
         <f>COUNTIF(D31:D35,"NA")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30">
@@ -11215,7 +11270,9 @@
       <c r="C32" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
@@ -11227,7 +11284,9 @@
       <c r="C33" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
@@ -11239,7 +11298,9 @@
       <c r="C34" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
@@ -11251,7 +11312,9 @@
       <c r="C35" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
@@ -11275,12 +11338,14 @@
       <c r="C37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
       <c r="G37">
         <f>COUNTIF(D37:D39,"Sim")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37">
         <f>COUNTIF(D37:D39,"Parcialmente")</f>
@@ -11303,7 +11368,9 @@
       <c r="C38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
@@ -11315,7 +11382,9 @@
       <c r="C39" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
@@ -11325,7 +11394,9 @@
       <c r="C40" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
@@ -11347,16 +11418,18 @@
       <c r="C42" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3" t="s">
+        <v>113</v>
+      </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42">
         <f>COUNTIF(D42:D43,"Sim")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <f>COUNTIF(D42:D43,"Parcialmente")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
         <f>COUNTIF(D42:D43,"Não")</f>
@@ -11375,7 +11448,9 @@
       <c r="C43" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
@@ -11409,6 +11484,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A30:A35"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A25:A29"/>
     <mergeCell ref="A5:A14"/>
     <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:F1"/>
@@ -11416,17 +11496,12 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A30:A35"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="A17:A21"/>
-    <mergeCell ref="A25:A29"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D25 D17 D15 D22 D41 D36 D30 D28" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Sim,Não,NA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D10:D12 D14 D16 D23:D24 D26:D27 D29 D31:D35 D42:D43 D18:D21 D37:D40" xr:uid="{00000000-0002-0000-0500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D8 D31:D35 D14 D10:D12 D26:D27 D18:D21 D29 D23:D24 D37:D40 D16 D42:D43" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"Sim,Parcialmente,Não,NA"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>